<commit_message>
Fast update on row and cell update fixing
</commit_message>
<xml_diff>
--- a/lisha1.00/bugs/screenshot/screenshots.xlsx
+++ b/lisha1.00/bugs/screenshot/screenshots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25020" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="28560" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12824,6 +12824,201 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>1689</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>1694</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="206" name="Image 205"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId66"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="321767200"/>
+          <a:ext cx="12077700" cy="1079500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>1691</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>1692</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="208" name="Rectangle 207"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6921500" y="322160900"/>
+          <a:ext cx="1054100" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>379482</xdr:colOff>
+      <xdr:row>1687</xdr:row>
+      <xdr:rowOff>121959</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>56763</xdr:colOff>
+      <xdr:row>1695</xdr:row>
+      <xdr:rowOff>134749</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="209" name="Flèche en arc 208"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="7808982" y="321495459"/>
+          <a:ext cx="3804781" cy="1536790"/>
+        </a:xfrm>
+        <a:prstGeom prst="circularArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 5574"/>
+            <a:gd name="adj2" fmla="val 633924"/>
+            <a:gd name="adj3" fmla="val 20747105"/>
+            <a:gd name="adj4" fmla="val 10800000"/>
+            <a:gd name="adj5" fmla="val 2787"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -13156,8 +13351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1660" workbookViewId="0">
-      <selection activeCell="O1672" sqref="O1672"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1671" workbookViewId="0">
+      <selection activeCell="Q1683" sqref="Q1683"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Background css fix and js comments
</commit_message>
<xml_diff>
--- a/lisha1.00/bugs/screenshot/screenshots.xlsx
+++ b/lisha1.00/bugs/screenshot/screenshots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="28560" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="21520" windowHeight="17200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -13022,6 +13022,51 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>1700</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>1721</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="210" name="Image 209"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId67"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1282700" y="323938900"/>
+          <a:ext cx="4940300" cy="4038600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -13351,7 +13396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1671" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1689" workbookViewId="0">
       <selection activeCell="Q1683" sqref="Q1683"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix utf8 issue on cell update for specific server configuration Force Json protection Use another way of htmlentities protection
</commit_message>
<xml_diff>
--- a/lisha1.00/bugs/screenshot/screenshots.xlsx
+++ b/lisha1.00/bugs/screenshot/screenshots.xlsx
@@ -13067,6 +13067,507 @@
         </a:effectLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>1707</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>1723</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="211" name="Image 210"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId68"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8242300" y="325285100"/>
+          <a:ext cx="8356600" cy="3124200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>1707</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>1710</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="212" name="Rectangle 211"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8509000" y="325361300"/>
+          <a:ext cx="3670300" cy="520700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>1705</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>1707</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="213" name="Ellipse 212"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11798300" y="324942200"/>
+          <a:ext cx="444500" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>1718</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>1721</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="214" name="Rectangle 213"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8394700" y="327367900"/>
+          <a:ext cx="2057400" cy="546100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>1716</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>1718</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="215" name="Ellipse 214"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10388600" y="326999600"/>
+          <a:ext cx="444500" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>B</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>1716</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>1720</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="216" name="Rectangle 215"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12369800" y="326936100"/>
+          <a:ext cx="3467100" cy="825500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1716</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>1718</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="217" name="Ellipse 216"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15875000" y="326923400"/>
+          <a:ext cx="444500" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -13396,8 +13897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1689" workbookViewId="0">
-      <selection activeCell="Q1683" sqref="Q1683"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1698" workbookViewId="0">
+      <selection activeCell="U1703" sqref="U1703"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Column option on update mode limitation Localized number on tool navigation bar
</commit_message>
<xml_diff>
--- a/lisha1.00/bugs/screenshot/screenshots.xlsx
+++ b/lisha1.00/bugs/screenshot/screenshots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="21520" windowHeight="17200" tabRatio="500"/>
+    <workbookView xWindow="100" yWindow="40" windowWidth="21520" windowHeight="17200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -13565,6 +13565,124 @@
             </a:rPr>
             <a:t>C</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>1734</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>1738</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="218" name="Image 217"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId69"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4419600" y="330352400"/>
+          <a:ext cx="1295400" cy="889000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>1735</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>1737</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="219" name="Ellipse 218"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5372100" y="330619100"/>
+          <a:ext cx="330200" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -13897,8 +14015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1698" workbookViewId="0">
-      <selection activeCell="U1703" sqref="U1703"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1721" workbookViewId="0">
+      <selection activeCell="H1736" sqref="H1736"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Export performance and limit
</commit_message>
<xml_diff>
--- a/lisha1.00/bugs/screenshot/screenshots.xlsx
+++ b/lisha1.00/bugs/screenshot/screenshots.xlsx
@@ -13683,6 +13683,260 @@
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>1730</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>1752</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="220" name="Image 219"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId70"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8356600" y="329742800"/>
+          <a:ext cx="2044700" cy="4013200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>1734</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>1740</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="221" name="Rectangle 220"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9220200" y="330454000"/>
+          <a:ext cx="863600" cy="1193800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1743</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1751</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="222" name="Rectangle 221"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9118600" y="332117700"/>
+          <a:ext cx="863600" cy="1473200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>122188</xdr:colOff>
+      <xdr:row>1735</xdr:row>
+      <xdr:rowOff>176108</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>332895</xdr:colOff>
+      <xdr:row>1736</xdr:row>
+      <xdr:rowOff>158909</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="223" name="Flèche vers la gauche 222"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19034225">
+          <a:off x="10028188" y="330693608"/>
+          <a:ext cx="1036207" cy="173301"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -14015,8 +14269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1721" workbookViewId="0">
-      <selection activeCell="H1736" sqref="H1736"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1722" workbookViewId="0">
+      <selection activeCell="H1738" sqref="H1738"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
quick search bug fix on log column
</commit_message>
<xml_diff>
--- a/lisha1.00/bugs/screenshot/screenshots.xlsx
+++ b/lisha1.00/bugs/screenshot/screenshots.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="40" windowWidth="21520" windowHeight="17200" tabRatio="500"/>
@@ -13937,6 +13937,197 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>1749</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>1755</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="224" name="Image 223"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId71"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3670300" y="333273400"/>
+          <a:ext cx="3581400" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>1750</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>1752</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="225" name="Ellipse 224"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4483100" y="333463900"/>
+          <a:ext cx="330200" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>1750</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1752</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="226" name="Ellipse 225"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6350000" y="333489300"/>
+          <a:ext cx="330200" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -14269,8 +14460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1722" workbookViewId="0">
-      <selection activeCell="H1738" sqref="H1738"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1727" workbookViewId="0">
+      <selection activeCell="J1740" sqref="J1740"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>